<commit_message>
added forgot password page and register page
</commit_message>
<xml_diff>
--- a/DB/CI_Platform_database_design.xlsx
+++ b/DB/CI_Platform_database_design.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="109">
   <si>
     <t>Field</t>
   </si>
@@ -337,6 +337,12 @@
   </si>
   <si>
     <t>goal_complete</t>
+  </si>
+  <si>
+    <t>hours</t>
+  </si>
+  <si>
+    <t>minutes</t>
   </si>
 </sst>
 </file>
@@ -809,10 +815,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A3:I136"/>
+  <dimension ref="A3:I138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="E136" sqref="E136"/>
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="G138" sqref="G138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3252,6 +3258,46 @@
       <c r="G136" s="4"/>
       <c r="H136" s="4"/>
       <c r="I136" s="4"/>
+    </row>
+    <row r="137" spans="1:9">
+      <c r="B137" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="C137" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D137" s="4">
+        <v>4</v>
+      </c>
+      <c r="E137" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F137" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G137" s="4"/>
+      <c r="H137" s="4"/>
+      <c r="I137" s="4"/>
+    </row>
+    <row r="138" spans="1:9">
+      <c r="B138" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="C138" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D138" s="4">
+        <v>4</v>
+      </c>
+      <c r="E138" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F138" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G138" s="4"/>
+      <c r="H138" s="4"/>
+      <c r="I138" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>